<commit_message>
Mise à jour des autorisations
</commit_message>
<xml_diff>
--- a/etml-gestgrades.xlsx
+++ b/etml-gestgrades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pe04uhp\Documents\GitHub\excel-etmlGrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32257386-633F-4D88-9F51-8855BB319B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E3CF20-BCA3-4502-97CC-B2320D003FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1ère année" sheetId="2" r:id="rId1"/>
@@ -626,6 +626,48 @@
     <xf numFmtId="2" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -651,48 +693,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -2076,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760258F2-7B94-4B16-858B-45F92CCB63C8}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2098,17 +2098,17 @@
   <sheetData>
     <row r="1" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -2132,42 +2132,42 @@
     </row>
     <row r="2" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="14"/>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="46" t="s">
+      <c r="N2" s="44"/>
+      <c r="O2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="47"/>
-      <c r="S2" s="46" t="s">
+      <c r="R2" s="44"/>
+      <c r="S2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="U2" s="51" t="s">
+      <c r="T2" s="44"/>
+      <c r="U2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="53"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="47"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
@@ -2178,43 +2178,43 @@
     </row>
     <row r="3" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
       <c r="K3" s="14"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="54">
+      <c r="L3" s="59"/>
+      <c r="M3" s="48">
         <f>IFERROR(AVERAGE(D6:E23),"DONNÉES INVALDES")</f>
         <v>3</v>
       </c>
-      <c r="N3" s="55"/>
-      <c r="O3" s="54">
+      <c r="N3" s="49"/>
+      <c r="O3" s="48">
         <f>IFERROR(AVERAGE(C6:C23),"NO DATA")</f>
         <v>6</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="54" cm="1">
+      <c r="P3" s="49"/>
+      <c r="Q3" s="48" cm="1">
         <f t="array" ref="Q3">IFERROR(((SUMPRODUCT(((I6:I23="A") + (I6:I23="LA")  + (I6:I23="#"))*J6:J23) / SUM(J6:J23)) * 100),"NO DATA")</f>
         <v>65.811965811965806</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="54">
+      <c r="R3" s="49"/>
+      <c r="S3" s="48">
         <f>IFERROR(AVERAGE(V5,V6,V7,V8,V10,V11,V12,V13,V15,V16,V17,V18,V20,V21,V22,V23),"INVALIDE")</f>
         <v>4.7</v>
       </c>
-      <c r="T3" s="55"/>
-      <c r="U3" s="54">
+      <c r="T3" s="49"/>
+      <c r="U3" s="48">
         <f>IFERROR(SUM((O3*10/100)+(M3*20/100)+(S3*30/100))/60*100,"DONNÉES INVALDES")</f>
         <v>4.3499999999999996</v>
       </c>
-      <c r="V3" s="56"/>
-      <c r="W3" s="55"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="49"/>
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="5" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -2274,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="37" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="17" t="s">
@@ -2287,7 +2287,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="14"/>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="40" t="s">
         <v>11</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -2336,7 +2336,7 @@
     </row>
     <row r="6" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="58"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="4">
         <v>6</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="58"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>45</v>
       </c>
       <c r="K6" s="14"/>
-      <c r="L6" s="49"/>
+      <c r="L6" s="41"/>
       <c r="M6" s="4">
         <v>6</v>
       </c>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="7" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="58"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="58"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>32</v>
       </c>
       <c r="K7" s="14"/>
-      <c r="L7" s="49"/>
+      <c r="L7" s="41"/>
       <c r="M7" s="4">
         <v>4</v>
       </c>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="8" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
-      <c r="B8" s="58"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="58"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="14"/>
-      <c r="L8" s="50"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="8">
         <v>0</v>
       </c>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="9" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="58"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="58"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="10" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="58"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="58"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="4" t="s">
         <v>3</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="14"/>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="40" t="s">
         <v>12</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -2662,7 +2662,7 @@
     </row>
     <row r="11" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="58"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="58"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="4" t="s">
         <v>3</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="14"/>
-      <c r="L11" s="49"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="4" t="s">
         <v>3</v>
       </c>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="12" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="58"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="4" t="s">
         <v>3</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="58"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="4" t="s">
         <v>3</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="14"/>
-      <c r="L12" s="49"/>
+      <c r="L12" s="41"/>
       <c r="M12" s="4" t="s">
         <v>3</v>
       </c>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="13" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="59"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="4" t="s">
         <v>3</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="59"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="14"/>
-      <c r="L13" s="50"/>
+      <c r="L13" s="42"/>
       <c r="M13" s="8" t="s">
         <v>3</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="14"/>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="40" t="s">
         <v>13</v>
       </c>
       <c r="M15" s="2" t="s">
@@ -3010,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="14"/>
-      <c r="L16" s="49"/>
+      <c r="L16" s="41"/>
       <c r="M16" s="4" t="s">
         <v>3</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="14"/>
-      <c r="L17" s="49"/>
+      <c r="L17" s="41"/>
       <c r="M17" s="4" t="s">
         <v>3</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="14"/>
-      <c r="L18" s="50"/>
+      <c r="L18" s="42"/>
       <c r="M18" s="8" t="s">
         <v>3</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="14"/>
-      <c r="L20" s="48" t="s">
+      <c r="L20" s="40" t="s">
         <v>14</v>
       </c>
       <c r="M20" s="2" t="s">
@@ -3336,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="14"/>
-      <c r="L21" s="49"/>
+      <c r="L21" s="41"/>
       <c r="M21" s="4" t="s">
         <v>3</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="14"/>
-      <c r="L22" s="49"/>
+      <c r="L22" s="41"/>
       <c r="M22" s="4" t="s">
         <v>3</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="14"/>
-      <c r="L23" s="50"/>
+      <c r="L23" s="42"/>
       <c r="M23" s="8" t="s">
         <v>3</v>
       </c>
@@ -3619,13 +3619,13 @@
       <c r="AD26" s="14"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="nieQ6Zieu7Wi/FksmO1fTvxcFVm0YqIm9+wwKlNIOSNmMiPi8sJ3nR1IF+m7L1EAbVWaFhn/sWmTAlcPEyX6XQ==" saltValue="1eBDg8Q5unzRLUQvi6p0lQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="5D90j6Ff/64U+AsZv+qyQHROmf/TWVJz2TJf66WqCZZLC4EFzLnI1BC6xKM4U3uYNnWNtVejDf8OH9UXu+K0jw==" saltValue="pahRCgzFcDYQlYOu98/9gA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="G5:G13"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:W2"/>
@@ -3635,11 +3635,11 @@
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="G5:G13"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="L15:L18"/>
   </mergeCells>
   <conditionalFormatting sqref="Q3:R3">
     <cfRule type="cellIs" dxfId="155" priority="46" operator="greaterThan">
@@ -3831,7 +3831,7 @@
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3852,17 +3852,17 @@
   <sheetData>
     <row r="1" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -3886,42 +3886,42 @@
     </row>
     <row r="2" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="14"/>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="46" t="s">
+      <c r="N2" s="44"/>
+      <c r="O2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="47"/>
-      <c r="S2" s="46" t="s">
+      <c r="R2" s="44"/>
+      <c r="S2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="U2" s="51" t="s">
+      <c r="T2" s="44"/>
+      <c r="U2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="53"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="47"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
@@ -3932,43 +3932,43 @@
     </row>
     <row r="3" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
       <c r="K3" s="14"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="54">
+      <c r="L3" s="59"/>
+      <c r="M3" s="48">
         <f>IFERROR(AVERAGE(D6:E23),"DONNÉES INVALDES")</f>
         <v>3</v>
       </c>
-      <c r="N3" s="55"/>
-      <c r="O3" s="54">
+      <c r="N3" s="49"/>
+      <c r="O3" s="48">
         <f>IFERROR(AVERAGE(C6:C23),"NO DATA")</f>
         <v>6</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="54" cm="1">
+      <c r="P3" s="49"/>
+      <c r="Q3" s="48" cm="1">
         <f t="array" ref="Q3">IFERROR(((SUMPRODUCT(((I6:I23="A") + (I6:I23="LA")  + (I6:I23="#"))*J6:J23) / SUM(J6:J23)) * 100),"NO DATA")</f>
         <v>65.811965811965806</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="54">
+      <c r="R3" s="49"/>
+      <c r="S3" s="48">
         <f>IFERROR(AVERAGE(V5,V6,V7,V8,V10,V11,V12,V13,V15,V16,V17,V18,V20,V21,V22,V23),"INVALIDE")</f>
         <v>4.7</v>
       </c>
-      <c r="T3" s="55"/>
-      <c r="U3" s="54">
+      <c r="T3" s="49"/>
+      <c r="U3" s="48">
         <f>IFERROR(SUM((O3*10/100)+(M3*20/100)+(S3*30/100))/60*100,"DONNÉES INVALDES")</f>
         <v>4.3499999999999996</v>
       </c>
-      <c r="V3" s="56"/>
-      <c r="W3" s="55"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="49"/>
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
@@ -4015,7 +4015,7 @@
     </row>
     <row r="5" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -4028,7 +4028,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="37" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="17" t="s">
@@ -4041,7 +4041,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="14"/>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="40" t="s">
         <v>11</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -4090,7 +4090,7 @@
     </row>
     <row r="6" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="58"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="4">
         <v>6</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="58"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>45</v>
       </c>
       <c r="K6" s="14"/>
-      <c r="L6" s="49"/>
+      <c r="L6" s="41"/>
       <c r="M6" s="4">
         <v>6</v>
       </c>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="7" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="58"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="58"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>32</v>
       </c>
       <c r="K7" s="14"/>
-      <c r="L7" s="49"/>
+      <c r="L7" s="41"/>
       <c r="M7" s="4">
         <v>4</v>
       </c>
@@ -4228,7 +4228,7 @@
     </row>
     <row r="8" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
-      <c r="B8" s="58"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="58"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="14"/>
-      <c r="L8" s="50"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="8">
         <v>0</v>
       </c>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="9" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="58"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="58"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="10" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="58"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="58"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="4" t="s">
         <v>3</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="14"/>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="40" t="s">
         <v>12</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -4416,7 +4416,7 @@
     </row>
     <row r="11" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="58"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="58"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="4" t="s">
         <v>3</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="14"/>
-      <c r="L11" s="49"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="4" t="s">
         <v>3</v>
       </c>
@@ -4485,7 +4485,7 @@
     </row>
     <row r="12" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="58"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="4" t="s">
         <v>3</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="58"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="4" t="s">
         <v>3</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="14"/>
-      <c r="L12" s="49"/>
+      <c r="L12" s="41"/>
       <c r="M12" s="4" t="s">
         <v>3</v>
       </c>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="13" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="59"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="4" t="s">
         <v>3</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="59"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="14"/>
-      <c r="L13" s="50"/>
+      <c r="L13" s="42"/>
       <c r="M13" s="8" t="s">
         <v>3</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="14"/>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="40" t="s">
         <v>13</v>
       </c>
       <c r="M15" s="2" t="s">
@@ -4764,7 +4764,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="14"/>
-      <c r="L16" s="49"/>
+      <c r="L16" s="41"/>
       <c r="M16" s="4" t="s">
         <v>3</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="14"/>
-      <c r="L17" s="49"/>
+      <c r="L17" s="41"/>
       <c r="M17" s="4" t="s">
         <v>3</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="14"/>
-      <c r="L18" s="50"/>
+      <c r="L18" s="42"/>
       <c r="M18" s="8" t="s">
         <v>3</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="14"/>
-      <c r="L20" s="48" t="s">
+      <c r="L20" s="40" t="s">
         <v>14</v>
       </c>
       <c r="M20" s="2" t="s">
@@ -5090,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="14"/>
-      <c r="L21" s="49"/>
+      <c r="L21" s="41"/>
       <c r="M21" s="4" t="s">
         <v>3</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="14"/>
-      <c r="L22" s="49"/>
+      <c r="L22" s="41"/>
       <c r="M22" s="4" t="s">
         <v>3</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="14"/>
-      <c r="L23" s="50"/>
+      <c r="L23" s="42"/>
       <c r="M23" s="8" t="s">
         <v>3</v>
       </c>
@@ -5375,15 +5375,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="uSC9yfNMGhWIuH/J2eNjKQkkDVQZpbEx7SuarFZzdt+ZpdH4hDK8u2FbnbhOtuXfvZ9FYX6Sq7elLPPzhUaafA==" saltValue="7Kipz996blBw/lQwaYAAWQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
-    <mergeCell ref="L15:L18"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="B2:J3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="G5:G13"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L10:L13"/>
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="B1:J1"/>
@@ -5394,6 +5385,15 @@
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="G5:G13"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L10:L13"/>
   </mergeCells>
   <conditionalFormatting sqref="Q3:R3">
     <cfRule type="cellIs" dxfId="107" priority="46" operator="greaterThan">
@@ -5585,7 +5585,7 @@
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5606,17 +5606,17 @@
   <sheetData>
     <row r="1" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -5640,42 +5640,42 @@
     </row>
     <row r="2" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="14"/>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="46" t="s">
+      <c r="N2" s="44"/>
+      <c r="O2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="47"/>
-      <c r="S2" s="46" t="s">
+      <c r="R2" s="44"/>
+      <c r="S2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="U2" s="51" t="s">
+      <c r="T2" s="44"/>
+      <c r="U2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="53"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="47"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
@@ -5686,43 +5686,43 @@
     </row>
     <row r="3" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
       <c r="K3" s="14"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="54">
+      <c r="L3" s="59"/>
+      <c r="M3" s="48">
         <f>IFERROR(AVERAGE(D6:E23),"DONNÉES INVALDES")</f>
         <v>3</v>
       </c>
-      <c r="N3" s="55"/>
-      <c r="O3" s="54">
+      <c r="N3" s="49"/>
+      <c r="O3" s="48">
         <f>IFERROR(AVERAGE(C6:C23),"NO DATA")</f>
         <v>6</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="54" cm="1">
+      <c r="P3" s="49"/>
+      <c r="Q3" s="48" cm="1">
         <f t="array" ref="Q3">IFERROR(((SUMPRODUCT(((I6:I23="A") + (I6:I23="LA")  + (I6:I23="#"))*J6:J23) / SUM(J6:J23)) * 100),"NO DATA")</f>
         <v>65.811965811965806</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="54">
+      <c r="R3" s="49"/>
+      <c r="S3" s="48">
         <f>IFERROR(AVERAGE(V5,V6,V7,V8,V10,V11,V12,V13),"INVALIDE")</f>
         <v>4.7</v>
       </c>
-      <c r="T3" s="55"/>
-      <c r="U3" s="54">
+      <c r="T3" s="49"/>
+      <c r="U3" s="48">
         <f>IFERROR(SUM((O3*10/100)+(M3*20/100)+(S3*30/100))/60*100,"DONNÉES INVALDES")</f>
         <v>4.3499999999999996</v>
       </c>
-      <c r="V3" s="56"/>
-      <c r="W3" s="55"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="49"/>
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="5" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -5782,7 +5782,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="37" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="17" t="s">
@@ -5795,7 +5795,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="14"/>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="40" t="s">
         <v>11</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -5844,7 +5844,7 @@
     </row>
     <row r="6" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="58"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="4">
         <v>6</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="58"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>45</v>
       </c>
       <c r="K6" s="14"/>
-      <c r="L6" s="49"/>
+      <c r="L6" s="41"/>
       <c r="M6" s="4">
         <v>6</v>
       </c>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="7" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="58"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="58"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>32</v>
       </c>
       <c r="K7" s="14"/>
-      <c r="L7" s="49"/>
+      <c r="L7" s="41"/>
       <c r="M7" s="4">
         <v>4</v>
       </c>
@@ -5982,7 +5982,7 @@
     </row>
     <row r="8" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
-      <c r="B8" s="58"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="58"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="14"/>
-      <c r="L8" s="50"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="8">
         <v>0</v>
       </c>
@@ -6051,7 +6051,7 @@
     </row>
     <row r="9" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="58"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="58"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
@@ -6099,7 +6099,7 @@
     </row>
     <row r="10" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="58"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="58"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="4" t="s">
         <v>3</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="14"/>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="40" t="s">
         <v>12</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -6170,7 +6170,7 @@
     </row>
     <row r="11" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="58"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="58"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="4" t="s">
         <v>3</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="14"/>
-      <c r="L11" s="49"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="4" t="s">
         <v>3</v>
       </c>
@@ -6239,7 +6239,7 @@
     </row>
     <row r="12" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="58"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="4" t="s">
         <v>3</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="58"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="4" t="s">
         <v>3</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="14"/>
-      <c r="L12" s="49"/>
+      <c r="L12" s="41"/>
       <c r="M12" s="4" t="s">
         <v>3</v>
       </c>
@@ -6308,7 +6308,7 @@
     </row>
     <row r="13" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="59"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="4" t="s">
         <v>3</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="59"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="14"/>
-      <c r="L13" s="50"/>
+      <c r="L13" s="42"/>
       <c r="M13" s="8" t="s">
         <v>3</v>
       </c>
@@ -6866,11 +6866,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="YSoMInjr8hludrfAgoxvqAJWvAbPr6WkedKAv1gNPcPhdrLyZqoiyv7+S1XFjquOZoQ/B46HkYFap7EZ8plQwA==" saltValue="QH7ZX1WwfIt1VuQrXQiXhg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="17">
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="G5:G13"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
@@ -6878,11 +6878,11 @@
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="G5:G13"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <conditionalFormatting sqref="Q3:R3">
     <cfRule type="cellIs" dxfId="59" priority="46" operator="greaterThan">
@@ -7007,8 +7007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72C9A25-D461-49AD-AA9A-88C0D94AE713}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7029,17 +7029,17 @@
   <sheetData>
     <row r="1" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -7063,42 +7063,42 @@
     </row>
     <row r="2" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="14"/>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="46" t="s">
+      <c r="N2" s="44"/>
+      <c r="O2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="47"/>
-      <c r="S2" s="46" t="s">
+      <c r="R2" s="44"/>
+      <c r="S2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="U2" s="51" t="s">
+      <c r="T2" s="44"/>
+      <c r="U2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="53"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="47"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
@@ -7109,43 +7109,43 @@
     </row>
     <row r="3" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
       <c r="K3" s="14"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="54">
+      <c r="L3" s="59"/>
+      <c r="M3" s="48">
         <f>IFERROR(AVERAGE(D6:E23),"DONNÉES INVALDES")</f>
         <v>3</v>
       </c>
-      <c r="N3" s="55"/>
-      <c r="O3" s="54">
+      <c r="N3" s="49"/>
+      <c r="O3" s="48">
         <f>IFERROR(AVERAGE(C6:C23),"NO DATA")</f>
         <v>6</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="54" cm="1">
+      <c r="P3" s="49"/>
+      <c r="Q3" s="48" cm="1">
         <f t="array" ref="Q3">IFERROR(((SUMPRODUCT(((I6:I23="A") + (I6:I23="LA")  + (I6:I23="#"))*J6:J23) / SUM(J6:J23)) * 100),"NO DATA")</f>
         <v>65.811965811965806</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="54">
+      <c r="R3" s="49"/>
+      <c r="S3" s="48">
         <f>IFERROR(AVERAGE(V5,V6,V7,V8,V10,V11,V12,V13),"INVALIDE")</f>
         <v>4.7</v>
       </c>
-      <c r="T3" s="55"/>
-      <c r="U3" s="54">
+      <c r="T3" s="49"/>
+      <c r="U3" s="48">
         <f>IFERROR(SUM((O3*10/100)+(M3*20/100)+(S3*30/100))/60*100,"DONNÉES INVALDES")</f>
         <v>4.3499999999999996</v>
       </c>
-      <c r="V3" s="56"/>
-      <c r="W3" s="55"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="49"/>
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
@@ -7192,7 +7192,7 @@
     </row>
     <row r="5" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -7205,7 +7205,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="37" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="17" t="s">
@@ -7218,7 +7218,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="14"/>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="40" t="s">
         <v>13</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -7267,7 +7267,7 @@
     </row>
     <row r="6" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="58"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="4">
         <v>6</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="58"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>45</v>
       </c>
       <c r="K6" s="14"/>
-      <c r="L6" s="49"/>
+      <c r="L6" s="41"/>
       <c r="M6" s="4">
         <v>6</v>
       </c>
@@ -7336,7 +7336,7 @@
     </row>
     <row r="7" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="58"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="58"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>32</v>
       </c>
       <c r="K7" s="14"/>
-      <c r="L7" s="49"/>
+      <c r="L7" s="41"/>
       <c r="M7" s="4">
         <v>4</v>
       </c>
@@ -7405,7 +7405,7 @@
     </row>
     <row r="8" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
-      <c r="B8" s="58"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="58"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="14"/>
-      <c r="L8" s="50"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="8">
         <v>0</v>
       </c>
@@ -7474,7 +7474,7 @@
     </row>
     <row r="9" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="58"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="58"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
@@ -7522,7 +7522,7 @@
     </row>
     <row r="10" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="58"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="58"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="4" t="s">
         <v>3</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="14"/>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="40" t="s">
         <v>14</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -7593,7 +7593,7 @@
     </row>
     <row r="11" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="58"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="58"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="4" t="s">
         <v>3</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="14"/>
-      <c r="L11" s="49"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="4" t="s">
         <v>3</v>
       </c>
@@ -7662,7 +7662,7 @@
     </row>
     <row r="12" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="58"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="4" t="s">
         <v>3</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="58"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="4" t="s">
         <v>3</v>
       </c>
@@ -7684,7 +7684,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="14"/>
-      <c r="L12" s="49"/>
+      <c r="L12" s="41"/>
       <c r="M12" s="4" t="s">
         <v>3</v>
       </c>
@@ -7731,7 +7731,7 @@
     </row>
     <row r="13" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="59"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="4" t="s">
         <v>3</v>
       </c>
@@ -7742,7 +7742,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="59"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="14"/>
-      <c r="L13" s="50"/>
+      <c r="L13" s="42"/>
       <c r="M13" s="8" t="s">
         <v>3</v>
       </c>
@@ -8289,11 +8289,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ntDi/8uLGwOMePA6jUid4pRqnJJA7lRzW6Slbzrm46AcYKXDI7jLIBXXNfhloDM1Kxy88y3abXrWLSP1//qnRQ==" saltValue="bBgkrgdV6QX2xK7MLtq+Qw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="17">
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="G5:G13"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
@@ -8301,11 +8301,11 @@
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="G5:G13"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <conditionalFormatting sqref="Q3:R3">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="greaterThan">

</xml_diff>

<commit_message>
ui(name/align): Agrandissement du champ nom de projet et alignement des intitulés de moyennes
</commit_message>
<xml_diff>
--- a/etml-gestgrades.xlsx
+++ b/etml-gestgrades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matej\Bureau\excel-etmlGrades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pe04uhp\Desktop\excel-etmlGrades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C5749E-25C4-4686-B3A4-142C1552D486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA408D50-7E5D-4C19-8C54-B462BD410338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="1620" windowWidth="28110" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1ère année" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="42">
   <si>
     <t>ECG</t>
   </si>
@@ -187,7 +187,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">V2 Gestionnaire de notes &amp; projets         </t>
+      <t xml:space="preserve">Gestionnaire de notes &amp; projets         </t>
     </r>
     <r>
       <rPr>
@@ -200,9 +200,6 @@
       <t>ETML</t>
     </r>
   </si>
-  <si>
-    <t>C000</t>
-  </si>
 </sst>
 </file>
 
@@ -211,7 +208,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0\p"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,6 +651,48 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -676,52 +715,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1644,18 +1641,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760258F2-7B94-4B16-858B-45F92CCB63C8}">
   <dimension ref="B1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
     <col min="3" max="5" width="11.5703125" style="1"/>
     <col min="6" max="6" width="6.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="11.5703125" style="1"/>
+    <col min="8" max="8" width="17.28515625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.5703125" style="1"/>
     <col min="11" max="11" width="5" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
     <col min="13" max="21" width="11.5703125" style="1"/>
@@ -1664,72 +1662,72 @@
     <col min="24" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="2:26" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
       <c r="X1" s="35"/>
       <c r="Y1" s="35"/>
       <c r="Z1" s="35"/>
     </row>
-    <row r="2" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="50" t="s">
+      <c r="M2" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="48"/>
+      <c r="O2" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="50" t="s">
+      <c r="P2" s="48"/>
+      <c r="Q2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="50" t="s">
+      <c r="R2" s="48"/>
+      <c r="S2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="51"/>
-      <c r="U2" s="55" t="s">
+      <c r="T2" s="48"/>
+      <c r="U2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="56"/>
-      <c r="W2" s="57"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="51"/>
       <c r="X2" s="35"/>
       <c r="Y2" s="35" t="s">
         <v>39</v>
@@ -1739,44 +1737,44 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47"/>
+    <row r="3" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="58" t="str">
+      <c r="L3" s="63"/>
+      <c r="M3" s="52" t="str">
         <f>IFERROR(C23,"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="N3" s="59"/>
-      <c r="O3" s="58" t="str">
+      <c r="N3" s="53"/>
+      <c r="O3" s="52" t="str">
         <f>IFERROR(AVERAGE(D23:E23),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="58" t="str" cm="1">
+      <c r="P3" s="53"/>
+      <c r="Q3" s="52" t="str" cm="1">
         <f t="array" ref="Q3">IFERROR(((SUMPRODUCT(((I6:I23="A") + (I6:I23="LA")  + (I6:I23="#"))*J6:J23) / SUM(J6:J23)) * 100),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="58" t="str">
+      <c r="R3" s="53"/>
+      <c r="S3" s="52" t="str">
         <f>IFERROR(Z2,"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="T3" s="59"/>
-      <c r="U3" s="58" t="str">
+      <c r="T3" s="53"/>
+      <c r="U3" s="52" t="str">
         <f>IFERROR(SUM((3*S3+2*O3+M3)/6),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="V3" s="60"/>
-      <c r="W3" s="59"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="53"/>
       <c r="X3" s="35"/>
       <c r="Y3" s="35" t="s">
         <v>37</v>
@@ -1786,7 +1784,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="24" customHeight="1" thickBot="1">
+    <row r="4" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1822,8 +1820,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1836,7 +1834,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="41" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -1849,7 +1847,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="52" t="s">
+      <c r="L5" s="44" t="s">
         <v>9</v>
       </c>
       <c r="M5" s="18" t="s">
@@ -1892,8 +1890,8 @@
       <c r="Y5" s="35"/>
       <c r="Z5" s="35"/>
     </row>
-    <row r="6" spans="2:26" ht="24" customHeight="1">
-      <c r="B6" s="62"/>
+    <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42"/>
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
@@ -1904,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="62"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="9" t="s">
         <v>3</v>
       </c>
@@ -1915,7 +1913,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="53"/>
+      <c r="L6" s="45"/>
       <c r="M6" s="9" t="s">
         <v>3</v>
       </c>
@@ -1956,8 +1954,8 @@
       <c r="Y6" s="35"/>
       <c r="Z6" s="35"/>
     </row>
-    <row r="7" spans="2:26" ht="24" customHeight="1">
-      <c r="B7" s="62"/>
+    <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="42"/>
       <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
@@ -1968,7 +1966,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="62"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="9" t="s">
         <v>3</v>
       </c>
@@ -1979,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="53"/>
+      <c r="L7" s="45"/>
       <c r="M7" s="9" t="s">
         <v>3</v>
       </c>
@@ -2017,8 +2015,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B8" s="62"/>
+    <row r="8" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
@@ -2029,7 +2027,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="62"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="9" t="s">
         <v>3</v>
       </c>
@@ -2040,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="54"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="15" t="s">
         <v>3</v>
       </c>
@@ -2078,8 +2076,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B9" s="62"/>
+    <row r="9" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
@@ -2090,7 +2088,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="62"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="9" t="s">
         <v>3</v>
       </c>
@@ -2118,8 +2116,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:26" ht="24" customHeight="1">
-      <c r="B10" s="62"/>
+    <row r="10" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="42"/>
       <c r="C10" s="9" t="s">
         <v>3</v>
       </c>
@@ -2130,7 +2128,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="62"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="9" t="s">
         <v>3</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="2"/>
-      <c r="L10" s="52" t="s">
+      <c r="L10" s="44" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="18" t="s">
@@ -2181,8 +2179,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="11" spans="2:26" ht="24" customHeight="1">
-      <c r="B11" s="62"/>
+    <row r="11" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="42"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
@@ -2193,7 +2191,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="62"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="9" t="s">
         <v>3</v>
       </c>
@@ -2204,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="53"/>
+      <c r="L11" s="45"/>
       <c r="M11" s="9" t="s">
         <v>3</v>
       </c>
@@ -2242,8 +2240,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="12" spans="2:26" ht="24" customHeight="1">
-      <c r="B12" s="62"/>
+    <row r="12" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="42"/>
       <c r="C12" s="9" t="s">
         <v>3</v>
       </c>
@@ -2254,7 +2252,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="62"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="9" t="s">
         <v>3</v>
       </c>
@@ -2265,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="53"/>
+      <c r="L12" s="45"/>
       <c r="M12" s="9" t="s">
         <v>3</v>
       </c>
@@ -2303,8 +2301,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="13" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B13" s="63"/>
+    <row r="13" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="43"/>
       <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
@@ -2315,7 +2313,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="63"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="9" t="s">
         <v>3</v>
       </c>
@@ -2326,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="54"/>
+      <c r="L13" s="46"/>
       <c r="M13" s="15" t="s">
         <v>3</v>
       </c>
@@ -2364,7 +2362,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="14" spans="2:26" ht="24" customHeight="1" thickBot="1">
+    <row r="14" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="9" t="s">
         <v>3</v>
@@ -2404,7 +2402,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:26" ht="24" customHeight="1">
+    <row r="15" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="9" t="s">
         <v>3</v>
@@ -2427,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="52" t="s">
+      <c r="L15" s="44" t="s">
         <v>11</v>
       </c>
       <c r="M15" s="18" t="s">
@@ -2467,7 +2465,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="16" spans="2:26" ht="24" customHeight="1">
+    <row r="16" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -2490,7 +2488,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="53"/>
+      <c r="L16" s="45"/>
       <c r="M16" s="9" t="s">
         <v>3</v>
       </c>
@@ -2528,7 +2526,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="17" spans="2:23" ht="24" customHeight="1">
+    <row r="17" spans="2:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
@@ -2551,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="L17" s="53"/>
+      <c r="L17" s="45"/>
       <c r="M17" s="9" t="s">
         <v>3</v>
       </c>
@@ -2589,7 +2587,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="18" spans="2:23" ht="24" customHeight="1" thickBot="1">
+    <row r="18" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="9" t="s">
         <v>3</v>
@@ -2612,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="54"/>
+      <c r="L18" s="46"/>
       <c r="M18" s="15" t="s">
         <v>3</v>
       </c>
@@ -2650,7 +2648,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="19" spans="2:23" ht="24" customHeight="1" thickBot="1">
+    <row r="19" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="9" t="s">
         <v>3</v>
@@ -2690,7 +2688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:23" ht="24" customHeight="1">
+    <row r="20" spans="2:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="9" t="s">
         <v>3</v>
@@ -2713,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="52" t="s">
+      <c r="L20" s="44" t="s">
         <v>12</v>
       </c>
       <c r="M20" s="18" t="s">
@@ -2753,7 +2751,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="21" spans="2:23" ht="24" customHeight="1">
+    <row r="21" spans="2:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="9" t="s">
         <v>3</v>
@@ -2776,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="53"/>
+      <c r="L21" s="45"/>
       <c r="M21" s="9" t="s">
         <v>3</v>
       </c>
@@ -2814,7 +2812,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="22" spans="2:23" ht="24" customHeight="1" thickBot="1">
+    <row r="22" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="9" t="s">
         <v>3</v>
@@ -2837,7 +2835,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="2"/>
-      <c r="L22" s="53"/>
+      <c r="L22" s="45"/>
       <c r="M22" s="9" t="s">
         <v>3</v>
       </c>
@@ -2875,7 +2873,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="23" spans="2:23" ht="24" customHeight="1" thickBot="1">
+    <row r="23" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="12" t="str">
         <f>IFERROR(ROUND(AVERAGE(C6:C22),1),"NO DATA")</f>
@@ -2901,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="2"/>
-      <c r="L23" s="54"/>
+      <c r="L23" s="46"/>
       <c r="M23" s="15" t="s">
         <v>3</v>
       </c>
@@ -2940,13 +2938,13 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="P2lDCqtM9r73z3X3G2Xbx4A2HnQAr+/0wJLe6FK0TxuKGGtdYTwhStChhv/P4ina03esNzY1LwMLBjicpEkYPg==" saltValue="5mNZ6xbatYHSl/nn8XYaXg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TXTs/GveCF+qwzjBOqjT5fdBpH+rq0WlNiq3RG6anQKJ649lEdc2E4ZsB+5+dFCJg7P6ZyClXtOC6FmplyMQXQ==" saltValue="8lqzu/McVmBfP1QwuafgUg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="G5:G13"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:W2"/>
@@ -2956,11 +2954,11 @@
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="B1:W1"/>
-    <mergeCell ref="B2:J3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="G5:G13"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="L15:L18"/>
   </mergeCells>
   <conditionalFormatting sqref="C23:E23">
     <cfRule type="cellIs" dxfId="87" priority="41" operator="equal">
@@ -3066,14 +3064,15 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
     <col min="3" max="5" width="11.5703125" style="1"/>
     <col min="6" max="6" width="6.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="11.5703125" style="1"/>
+    <col min="8" max="8" width="17.28515625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.5703125" style="1"/>
     <col min="11" max="11" width="5" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
     <col min="13" max="21" width="11.5703125" style="1"/>
@@ -3082,72 +3081,72 @@
     <col min="24" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="2:26" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
       <c r="X1" s="35"/>
       <c r="Y1" s="35"/>
       <c r="Z1" s="35"/>
     </row>
-    <row r="2" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="50" t="s">
+      <c r="M2" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="48"/>
+      <c r="O2" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="50" t="s">
+      <c r="P2" s="48"/>
+      <c r="Q2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="50" t="s">
+      <c r="R2" s="48"/>
+      <c r="S2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="51"/>
-      <c r="U2" s="55" t="s">
+      <c r="T2" s="48"/>
+      <c r="U2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="56"/>
-      <c r="W2" s="57"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="51"/>
       <c r="X2" s="35"/>
       <c r="Y2" s="35" t="s">
         <v>39</v>
@@ -3157,44 +3156,44 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47"/>
+    <row r="3" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="58" t="str">
+      <c r="L3" s="63"/>
+      <c r="M3" s="52" t="str">
         <f>IFERROR(C23,"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="N3" s="59"/>
-      <c r="O3" s="58" t="str">
+      <c r="N3" s="53"/>
+      <c r="O3" s="52" t="str">
         <f>IFERROR(AVERAGE(D23:E23),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="58" t="str" cm="1">
+      <c r="P3" s="53"/>
+      <c r="Q3" s="52" t="str" cm="1">
         <f t="array" ref="Q3">IFERROR(((SUMPRODUCT(((I6:I23="A") + (I6:I23="LA")  + (I6:I23="#"))*J6:J23) / SUM(J6:J23)) * 100),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="58" t="str">
+      <c r="R3" s="53"/>
+      <c r="S3" s="52" t="str">
         <f>IFERROR(Z2,"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="T3" s="59"/>
-      <c r="U3" s="58" t="str">
+      <c r="T3" s="53"/>
+      <c r="U3" s="52" t="str">
         <f>IFERROR(SUM((3*S3+2*O3+M3)/6),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="V3" s="60"/>
-      <c r="W3" s="59"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="53"/>
       <c r="X3" s="35"/>
       <c r="Y3" s="35" t="s">
         <v>37</v>
@@ -3204,7 +3203,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="24" customHeight="1" thickBot="1">
+    <row r="4" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3240,8 +3239,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -3254,7 +3253,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="41" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -3267,11 +3266,11 @@
         <v>8</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="52" t="s">
+      <c r="L5" s="44" t="s">
         <v>9</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="N5" s="8" t="s">
         <v>13</v>
@@ -3296,7 +3295,7 @@
       </c>
       <c r="U5" s="19" t="str">
         <f>M5</f>
-        <v>C000</v>
+        <v>I001</v>
       </c>
       <c r="V5" s="20" t="str">
         <f>IFERROR((M6*N6 + M7*N7 + M8*N8), "INVALIDE")</f>
@@ -3310,8 +3309,8 @@
       <c r="Y5" s="35"/>
       <c r="Z5" s="35"/>
     </row>
-    <row r="6" spans="2:26" ht="24" customHeight="1">
-      <c r="B6" s="62"/>
+    <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42"/>
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
@@ -3322,7 +3321,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="62"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="9" t="s">
         <v>3</v>
       </c>
@@ -3333,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="53"/>
+      <c r="L6" s="45"/>
       <c r="M6" s="9" t="s">
         <v>3</v>
       </c>
@@ -3374,8 +3373,8 @@
       <c r="Y6" s="35"/>
       <c r="Z6" s="35"/>
     </row>
-    <row r="7" spans="2:26" ht="24" customHeight="1">
-      <c r="B7" s="62"/>
+    <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="42"/>
       <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
@@ -3386,7 +3385,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="62"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="9" t="s">
         <v>3</v>
       </c>
@@ -3397,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="53"/>
+      <c r="L7" s="45"/>
       <c r="M7" s="9" t="s">
         <v>3</v>
       </c>
@@ -3435,8 +3434,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B8" s="62"/>
+    <row r="8" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
@@ -3447,7 +3446,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="62"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="9" t="s">
         <v>3</v>
       </c>
@@ -3458,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="54"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="15" t="s">
         <v>3</v>
       </c>
@@ -3496,8 +3495,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B9" s="62"/>
+    <row r="9" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="62"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="9" t="s">
         <v>3</v>
       </c>
@@ -3536,8 +3535,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:26" ht="24" customHeight="1">
-      <c r="B10" s="62"/>
+    <row r="10" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="42"/>
       <c r="C10" s="9" t="s">
         <v>3</v>
       </c>
@@ -3548,7 +3547,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="62"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="9" t="s">
         <v>3</v>
       </c>
@@ -3559,7 +3558,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="2"/>
-      <c r="L10" s="52" t="s">
+      <c r="L10" s="44" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="18" t="s">
@@ -3599,8 +3598,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="11" spans="2:26" ht="24" customHeight="1">
-      <c r="B11" s="62"/>
+    <row r="11" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="42"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
@@ -3611,7 +3610,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="62"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="9" t="s">
         <v>3</v>
       </c>
@@ -3622,7 +3621,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="53"/>
+      <c r="L11" s="45"/>
       <c r="M11" s="9" t="s">
         <v>3</v>
       </c>
@@ -3660,8 +3659,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="12" spans="2:26" ht="24" customHeight="1">
-      <c r="B12" s="62"/>
+    <row r="12" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="42"/>
       <c r="C12" s="9" t="s">
         <v>3</v>
       </c>
@@ -3672,7 +3671,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="62"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="9" t="s">
         <v>3</v>
       </c>
@@ -3683,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="53"/>
+      <c r="L12" s="45"/>
       <c r="M12" s="9" t="s">
         <v>3</v>
       </c>
@@ -3721,8 +3720,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="13" spans="2:26" ht="24" customHeight="1" thickBot="1">
-      <c r="B13" s="63"/>
+    <row r="13" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="43"/>
       <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
@@ -3733,7 +3732,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="63"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="9" t="s">
         <v>3</v>
       </c>
@@ -3744,7 +3743,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="54"/>
+      <c r="L13" s="46"/>
       <c r="M13" s="15" t="s">
         <v>3</v>
       </c>
@@ -3782,7 +3781,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="14" spans="2:26" ht="24" customHeight="1" thickBot="1">
+    <row r="14" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="9" t="s">
         <v>3</v>
@@ -3822,7 +3821,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:26" ht="24" customHeight="1">
+    <row r="15" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="9" t="s">
         <v>3</v>
@@ -3845,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="52" t="s">
+      <c r="L15" s="44" t="s">
         <v>11</v>
       </c>
       <c r="M15" s="18" t="s">
@@ -3885,7 +3884,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="16" spans="2:26" ht="24" customHeight="1">
+    <row r="16" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -3908,7 +3907,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="53"/>
+      <c r="L16" s="45"/>
       <c r="M16" s="9" t="s">
         <v>3</v>
       </c>
@@ -3946,7 +3945,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="17" spans="2:23" ht="24" customHeight="1">
+    <row r="17" spans="2:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
@@ -3969,7 +3968,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="L17" s="53"/>
+      <c r="L17" s="45"/>
       <c r="M17" s="9" t="s">
         <v>3</v>
       </c>
@@ -4007,7 +4006,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="18" spans="2:23" ht="24" customHeight="1" thickBot="1">
+    <row r="18" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="9" t="s">
         <v>3</v>
@@ -4030,7 +4029,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="54"/>
+      <c r="L18" s="46"/>
       <c r="M18" s="15" t="s">
         <v>3</v>
       </c>
@@ -4068,7 +4067,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="19" spans="2:23" ht="24" customHeight="1" thickBot="1">
+    <row r="19" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="9" t="s">
         <v>3</v>
@@ -4108,7 +4107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:23" ht="24" customHeight="1">
+    <row r="20" spans="2:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="9" t="s">
         <v>3</v>
@@ -4131,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="52" t="s">
+      <c r="L20" s="44" t="s">
         <v>12</v>
       </c>
       <c r="M20" s="18" t="s">
@@ -4171,7 +4170,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="21" spans="2:23" ht="24" customHeight="1">
+    <row r="21" spans="2:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="9" t="s">
         <v>3</v>
@@ -4194,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="53"/>
+      <c r="L21" s="45"/>
       <c r="M21" s="9" t="s">
         <v>3</v>
       </c>
@@ -4232,7 +4231,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="22" spans="2:23" ht="24" customHeight="1" thickBot="1">
+    <row r="22" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="9" t="s">
         <v>3</v>
@@ -4255,7 +4254,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="2"/>
-      <c r="L22" s="53"/>
+      <c r="L22" s="45"/>
       <c r="M22" s="9" t="s">
         <v>3</v>
       </c>
@@ -4293,7 +4292,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="23" spans="2:23" ht="24" customHeight="1" thickBot="1">
+    <row r="23" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="12" t="str">
         <f>IFERROR(ROUND(AVERAGE(C6:C22),1),"NO DATA")</f>
@@ -4319,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="2"/>
-      <c r="L23" s="54"/>
+      <c r="L23" s="46"/>
       <c r="M23" s="15" t="s">
         <v>3</v>
       </c>
@@ -4358,8 +4357,13 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="BQHWkbsFYDJcLPIvBxCnqY1QYOeb6s6Kz8QfIgV/cgVGqWeVZljC9DZXGmrHbPXOMvG1nEYt5L1spXej4lqsfg==" saltValue="07J6pNibCEXT7znQN+wGQw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="C/EZJERaAq7nRBFX0qHQirccVumWoamRcftfiNo6yPQkF/3fCaCIZdJR0/1rG2uiMpxQdT+qYWL3CqoPTCUbWA==" saltValue="SomBY6gIMFcZ2KWNQaJIqA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
+    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:W3"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="G5:G13"/>
     <mergeCell ref="L5:L8"/>
@@ -4374,11 +4378,6 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
-    <mergeCell ref="L15:L18"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:W3"/>
   </mergeCells>
   <conditionalFormatting sqref="C23:E23">
     <cfRule type="cellIs" dxfId="62" priority="17" operator="equal">
@@ -4480,17 +4479,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB92B99-8C25-4EE0-9704-56C2693F154E}">
   <dimension ref="B1:AB23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
     <col min="3" max="5" width="11.5703125" style="1"/>
     <col min="6" max="6" width="6.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="1" customWidth="1"/>
     <col min="8" max="10" width="11.5703125" style="1"/>
     <col min="11" max="11" width="5" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
@@ -4500,74 +4499,74 @@
     <col min="24" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="2:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
       <c r="X1" s="35"/>
       <c r="Y1" s="35"/>
       <c r="Z1" s="35"/>
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
     </row>
-    <row r="2" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="50" t="s">
+      <c r="M2" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="48"/>
+      <c r="O2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="50" t="s">
+      <c r="P2" s="48"/>
+      <c r="Q2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="50" t="s">
+      <c r="R2" s="48"/>
+      <c r="S2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="51"/>
-      <c r="U2" s="55" t="s">
+      <c r="T2" s="48"/>
+      <c r="U2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="56"/>
-      <c r="W2" s="57"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="51"/>
       <c r="X2" s="35"/>
       <c r="Y2" s="35" t="s">
         <v>39</v>
@@ -4579,44 +4578,44 @@
       <c r="AA2" s="35"/>
       <c r="AB2" s="35"/>
     </row>
-    <row r="3" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47"/>
+    <row r="3" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="58" t="str">
+      <c r="L3" s="63"/>
+      <c r="M3" s="52" t="str">
         <f>IFERROR(C23,"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="N3" s="59"/>
-      <c r="O3" s="58" t="str">
+      <c r="N3" s="53"/>
+      <c r="O3" s="52" t="str">
         <f>IFERROR(AVERAGE(D23:E23),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="58" t="str" cm="1">
+      <c r="P3" s="53"/>
+      <c r="Q3" s="52" t="str" cm="1">
         <f t="array" ref="Q3">IFERROR(((SUMPRODUCT(((H6:H23="A") + (H6:H23="LA")  + (H6:H23="#"))*I6:I23) / SUM(I6:I23)) * 100),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="58" t="str">
+      <c r="R3" s="53"/>
+      <c r="S3" s="52" t="str">
         <f>IFERROR(Z2,"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="T3" s="59"/>
-      <c r="U3" s="58" t="str">
+      <c r="T3" s="53"/>
+      <c r="U3" s="52" t="str">
         <f>IFERROR(SUM((3*S3+2*O3+M3)/6),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="V3" s="60"/>
-      <c r="W3" s="59"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="53"/>
       <c r="X3" s="35"/>
       <c r="Y3" s="35" t="s">
         <v>37</v>
@@ -4628,7 +4627,7 @@
       <c r="AA3" s="35"/>
       <c r="AB3" s="35"/>
     </row>
-    <row r="4" spans="2:28" ht="24" customHeight="1" thickBot="1">
+    <row r="4" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -4666,8 +4665,8 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="35"/>
     </row>
-    <row r="5" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4677,7 +4676,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="38"/>
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="41" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -4690,7 +4689,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="52" t="s">
+      <c r="L5" s="44" t="s">
         <v>9</v>
       </c>
       <c r="M5" s="18" t="s">
@@ -4735,8 +4734,8 @@
       <c r="AA5" s="35"/>
       <c r="AB5" s="35"/>
     </row>
-    <row r="6" spans="2:28" ht="24" customHeight="1">
-      <c r="B6" s="62"/>
+    <row r="6" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42"/>
       <c r="C6" s="36" t="s">
         <v>3</v>
       </c>
@@ -4744,7 +4743,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="62"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="9" t="s">
         <v>3</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="53"/>
+      <c r="L6" s="45"/>
       <c r="M6" s="9" t="s">
         <v>3</v>
       </c>
@@ -4798,8 +4797,8 @@
       <c r="AA6" s="35"/>
       <c r="AB6" s="35"/>
     </row>
-    <row r="7" spans="2:28" ht="24" customHeight="1">
-      <c r="B7" s="62"/>
+    <row r="7" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="42"/>
       <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="62"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="9" t="s">
         <v>3</v>
       </c>
@@ -4818,7 +4817,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="53"/>
+      <c r="L7" s="45"/>
       <c r="M7" s="9" t="s">
         <v>3</v>
       </c>
@@ -4860,8 +4859,8 @@
       <c r="AA7" s="35"/>
       <c r="AB7" s="35"/>
     </row>
-    <row r="8" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B8" s="62"/>
+    <row r="8" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
@@ -4869,7 +4868,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="62"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="9" t="s">
         <v>3</v>
       </c>
@@ -4880,7 +4879,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="54"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="15" t="s">
         <v>3</v>
       </c>
@@ -4922,8 +4921,8 @@
       <c r="AA8" s="35"/>
       <c r="AB8" s="35"/>
     </row>
-    <row r="9" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B9" s="62"/>
+    <row r="9" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
@@ -4931,7 +4930,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="62"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="9" t="s">
         <v>3</v>
       </c>
@@ -4959,8 +4958,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:28" ht="24" customHeight="1">
-      <c r="B10" s="62"/>
+    <row r="10" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="42"/>
       <c r="C10" s="9" t="s">
         <v>3</v>
       </c>
@@ -4968,7 +4967,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="62"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="9" t="s">
         <v>3</v>
       </c>
@@ -4979,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="2"/>
-      <c r="L10" s="52" t="s">
+      <c r="L10" s="44" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="18" t="s">
@@ -5019,8 +5018,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="11" spans="2:28" ht="24" customHeight="1">
-      <c r="B11" s="62"/>
+    <row r="11" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="42"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
@@ -5028,7 +5027,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="62"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="9" t="s">
         <v>3</v>
       </c>
@@ -5039,7 +5038,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="53"/>
+      <c r="L11" s="45"/>
       <c r="M11" s="9" t="s">
         <v>3</v>
       </c>
@@ -5077,8 +5076,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="12" spans="2:28" ht="24" customHeight="1">
-      <c r="B12" s="62"/>
+    <row r="12" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="42"/>
       <c r="C12" s="9" t="s">
         <v>3</v>
       </c>
@@ -5086,7 +5085,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="62"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="9" t="s">
         <v>3</v>
       </c>
@@ -5097,7 +5096,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="53"/>
+      <c r="L12" s="45"/>
       <c r="M12" s="9" t="s">
         <v>3</v>
       </c>
@@ -5135,8 +5134,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="13" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B13" s="63"/>
+    <row r="13" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="43"/>
       <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
@@ -5144,7 +5143,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="63"/>
+      <c r="F13" s="43"/>
       <c r="G13" s="9" t="s">
         <v>3</v>
       </c>
@@ -5155,7 +5154,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="54"/>
+      <c r="L13" s="46"/>
       <c r="M13" s="15" t="s">
         <v>3</v>
       </c>
@@ -5193,7 +5192,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="14" spans="2:28" ht="24" customHeight="1">
+    <row r="14" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="9" t="s">
         <v>3</v>
@@ -5214,7 +5213,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:28" ht="24" customHeight="1">
+    <row r="15" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="9" t="s">
         <v>3</v>
@@ -5235,7 +5234,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="2:28" ht="24" customHeight="1">
+    <row r="16" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -5256,7 +5255,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="2:11" ht="24" customHeight="1">
+    <row r="17" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
@@ -5277,7 +5276,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="2:11" ht="24" customHeight="1">
+    <row r="18" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="9" t="s">
         <v>3</v>
@@ -5298,7 +5297,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="2:11" ht="24" customHeight="1">
+    <row r="19" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="9" t="s">
         <v>3</v>
@@ -5319,7 +5318,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="2:11" ht="24" customHeight="1">
+    <row r="20" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="9" t="s">
         <v>3</v>
@@ -5340,7 +5339,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="2:11" ht="24" customHeight="1">
+    <row r="21" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="9" t="s">
         <v>3</v>
@@ -5361,7 +5360,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="2:11" ht="24" customHeight="1" thickBot="1">
+    <row r="22" spans="2:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="9" t="s">
         <v>3</v>
@@ -5382,7 +5381,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="2:11" ht="24" customHeight="1" thickBot="1">
+    <row r="23" spans="2:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="12" t="str">
         <f>IFERROR(ROUND(AVERAGE(C6:C22),1),"NO DATA")</f>
@@ -5406,8 +5405,12 @@
       <c r="K23" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="k+fMWELo1rSaRBq1CdLP1pmFrgVSJd6x+fm9RCZxFvNcSDxA50knefHUf8zicp7pr6aJekam07MG34K67Kj4kg==" saltValue="qQ4wlBq4WvUY+yLxqJgV6w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dyUC2VLS86eXEI+0ceW8VKUiBi1P9XEbzGtUIIObrWzn41C877H3MJ+artChJplL4dg74k/0gh/GtiTZpnEv6g==" saltValue="K6EOxdpHGVVTwdyiWZ4HkA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="17">
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="F5:F13"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L10:L13"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="L2:L3"/>
@@ -5421,10 +5424,6 @@
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="U3:W3"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="F5:F13"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L10:L13"/>
   </mergeCells>
   <conditionalFormatting sqref="C23:D23">
     <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
@@ -5504,17 +5503,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61012CEC-844D-4C26-9DFB-9069EEAE3421}">
   <dimension ref="B1:AB23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
     <col min="3" max="5" width="11.5703125" style="1"/>
     <col min="6" max="6" width="6.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1"/>
     <col min="8" max="10" width="11.5703125" style="1"/>
     <col min="11" max="11" width="5" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
@@ -5524,74 +5523,74 @@
     <col min="24" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="2:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
       <c r="X1" s="35"/>
       <c r="Y1" s="35"/>
       <c r="Z1" s="35"/>
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
     </row>
-    <row r="2" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="50" t="s">
+      <c r="M2" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="48"/>
+      <c r="O2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="50" t="s">
+      <c r="P2" s="48"/>
+      <c r="Q2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="50" t="s">
+      <c r="R2" s="48"/>
+      <c r="S2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="51"/>
-      <c r="U2" s="55" t="s">
+      <c r="T2" s="48"/>
+      <c r="U2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="56"/>
-      <c r="W2" s="57"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="51"/>
       <c r="X2" s="35"/>
       <c r="Y2" s="35" t="s">
         <v>39</v>
@@ -5603,44 +5602,44 @@
       <c r="AA2" s="35"/>
       <c r="AB2" s="35"/>
     </row>
-    <row r="3" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47"/>
+    <row r="3" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="58" t="str">
+      <c r="L3" s="63"/>
+      <c r="M3" s="52" t="str">
         <f>IFERROR(C23,"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="N3" s="59"/>
-      <c r="O3" s="58" t="str">
+      <c r="N3" s="53"/>
+      <c r="O3" s="52" t="str">
         <f>IFERROR(AVERAGE(D23:E23),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="58" t="str" cm="1">
+      <c r="P3" s="53"/>
+      <c r="Q3" s="52" t="str" cm="1">
         <f t="array" ref="Q3">IFERROR(((SUMPRODUCT(((H6:H23="A") + (H6:H23="LA")  + (H6:H23="#"))*I6:I23) / SUM(I6:I23)) * 100),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="58" t="str">
+      <c r="R3" s="53"/>
+      <c r="S3" s="52" t="str">
         <f>IFERROR(Z2,"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="T3" s="59"/>
-      <c r="U3" s="58" t="str">
+      <c r="T3" s="53"/>
+      <c r="U3" s="52" t="str">
         <f>IFERROR(SUM((3*S3+2*O3+M3)/6),"NO DATA")</f>
         <v>NO DATA</v>
       </c>
-      <c r="V3" s="60"/>
-      <c r="W3" s="59"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="53"/>
       <c r="X3" s="35"/>
       <c r="Y3" s="35" t="s">
         <v>37</v>
@@ -5652,7 +5651,7 @@
       <c r="AA3" s="35"/>
       <c r="AB3" s="35"/>
     </row>
-    <row r="4" spans="2:28" ht="24" customHeight="1" thickBot="1">
+    <row r="4" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -5690,8 +5689,8 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="35"/>
     </row>
-    <row r="5" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -5701,7 +5700,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="38"/>
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="41" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -5714,7 +5713,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="52" t="s">
+      <c r="L5" s="44" t="s">
         <v>11</v>
       </c>
       <c r="M5" s="18" t="s">
@@ -5759,8 +5758,8 @@
       <c r="AA5" s="35"/>
       <c r="AB5" s="35"/>
     </row>
-    <row r="6" spans="2:28" ht="24" customHeight="1">
-      <c r="B6" s="62"/>
+    <row r="6" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42"/>
       <c r="C6" s="36" t="s">
         <v>3</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="62"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="9" t="s">
         <v>3</v>
       </c>
@@ -5779,7 +5778,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="53"/>
+      <c r="L6" s="45"/>
       <c r="M6" s="9" t="s">
         <v>3</v>
       </c>
@@ -5822,8 +5821,8 @@
       <c r="AA6" s="35"/>
       <c r="AB6" s="35"/>
     </row>
-    <row r="7" spans="2:28" ht="24" customHeight="1">
-      <c r="B7" s="62"/>
+    <row r="7" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="42"/>
       <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
@@ -5831,7 +5830,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="62"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="9" t="s">
         <v>3</v>
       </c>
@@ -5842,7 +5841,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="53"/>
+      <c r="L7" s="45"/>
       <c r="M7" s="9" t="s">
         <v>3</v>
       </c>
@@ -5884,8 +5883,8 @@
       <c r="AA7" s="35"/>
       <c r="AB7" s="35"/>
     </row>
-    <row r="8" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B8" s="62"/>
+    <row r="8" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
@@ -5893,7 +5892,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="62"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="9" t="s">
         <v>3</v>
       </c>
@@ -5904,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="54"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="15" t="s">
         <v>3</v>
       </c>
@@ -5946,8 +5945,8 @@
       <c r="AA8" s="35"/>
       <c r="AB8" s="35"/>
     </row>
-    <row r="9" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B9" s="62"/>
+    <row r="9" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
@@ -5955,7 +5954,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="62"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="9" t="s">
         <v>3</v>
       </c>
@@ -5983,8 +5982,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:28" ht="24" customHeight="1">
-      <c r="B10" s="62"/>
+    <row r="10" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="42"/>
       <c r="C10" s="9" t="s">
         <v>3</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="62"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="9" t="s">
         <v>3</v>
       </c>
@@ -6003,7 +6002,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="2"/>
-      <c r="L10" s="52" t="s">
+      <c r="L10" s="44" t="s">
         <v>12</v>
       </c>
       <c r="M10" s="18" t="s">
@@ -6043,8 +6042,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="11" spans="2:28" ht="24" customHeight="1">
-      <c r="B11" s="62"/>
+    <row r="11" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="42"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
@@ -6052,7 +6051,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="62"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="9" t="s">
         <v>3</v>
       </c>
@@ -6063,7 +6062,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="53"/>
+      <c r="L11" s="45"/>
       <c r="M11" s="9" t="s">
         <v>3</v>
       </c>
@@ -6101,8 +6100,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="12" spans="2:28" ht="24" customHeight="1">
-      <c r="B12" s="62"/>
+    <row r="12" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="42"/>
       <c r="C12" s="9" t="s">
         <v>3</v>
       </c>
@@ -6110,7 +6109,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="62"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="9" t="s">
         <v>3</v>
       </c>
@@ -6121,7 +6120,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="53"/>
+      <c r="L12" s="45"/>
       <c r="M12" s="9" t="s">
         <v>3</v>
       </c>
@@ -6159,8 +6158,8 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="13" spans="2:28" ht="24" customHeight="1" thickBot="1">
-      <c r="B13" s="63"/>
+    <row r="13" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="43"/>
       <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
@@ -6168,7 +6167,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="63"/>
+      <c r="F13" s="43"/>
       <c r="G13" s="9" t="s">
         <v>3</v>
       </c>
@@ -6179,7 +6178,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="54"/>
+      <c r="L13" s="46"/>
       <c r="M13" s="15" t="s">
         <v>3</v>
       </c>
@@ -6217,7 +6216,7 @@
         <v>INVALIDE</v>
       </c>
     </row>
-    <row r="14" spans="2:28" ht="24" customHeight="1">
+    <row r="14" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="9" t="s">
         <v>3</v>
@@ -6238,7 +6237,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:28" ht="24" customHeight="1">
+    <row r="15" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="9" t="s">
         <v>3</v>
@@ -6259,7 +6258,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="2:28" ht="24" customHeight="1">
+    <row r="16" spans="2:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -6280,7 +6279,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="2:11" ht="24" customHeight="1">
+    <row r="17" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
@@ -6301,7 +6300,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="2:11" ht="24" customHeight="1">
+    <row r="18" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="9" t="s">
         <v>3</v>
@@ -6322,7 +6321,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="2:11" ht="24" customHeight="1">
+    <row r="19" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="9" t="s">
         <v>3</v>
@@ -6343,7 +6342,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="2:11" ht="24" customHeight="1">
+    <row r="20" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="9" t="s">
         <v>3</v>
@@ -6364,7 +6363,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="2:11" ht="24" customHeight="1">
+    <row r="21" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="9" t="s">
         <v>3</v>
@@ -6385,7 +6384,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="2:11" ht="24" customHeight="1" thickBot="1">
+    <row r="22" spans="2:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="9" t="s">
         <v>3</v>
@@ -6406,7 +6405,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="2:11" ht="24" customHeight="1" thickBot="1">
+    <row r="23" spans="2:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="12" t="str">
         <f>IFERROR(ROUND(AVERAGE(C6:C22),1),"NO DATA")</f>
@@ -6430,8 +6429,12 @@
       <c r="K23" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bIi0xcUMJ0ol2uWbMKG5pIBFtT8MJw3q214RpvL/OFO1G9C0KXvOaltW21EbOYHHetEOotT0+cO6JacH4h/enQ==" saltValue="362YgO2a+TEiNne5WD9q6A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="n+Rww3lJqnvXhRaq+fxFaB6Bm89VhIX0s9q2Zan3MQ95ZuLzZmpieVmB744fgZOlMo11tFJBd48u0QYkm8KAUA==" saltValue="TdjtMz3VoDWWWmSaA7c1mw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="17">
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="F5:F13"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L10:L13"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="L2:L3"/>
@@ -6445,10 +6448,6 @@
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="U3:W3"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="F5:F13"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L10:L13"/>
   </mergeCells>
   <conditionalFormatting sqref="C23:D23">
     <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">

</xml_diff>